<commit_message>
Add panel (FE) pipeline + panel_summary in Excel; cross-ticker plot
</commit_message>
<xml_diff>
--- a/reports/summary.xlsx
+++ b/reports/summary.xlsx
@@ -15,14 +15,15 @@
     <sheet name="correlations_all" sheetId="6" r:id="rId6"/>
     <sheet name="events_all" sheetId="7" r:id="rId7"/>
     <sheet name="events_summary" sheetId="8" r:id="rId8"/>
-    <sheet name="README" sheetId="9" r:id="rId9"/>
+    <sheet name="panel_summary" sheetId="9" r:id="rId9"/>
+    <sheet name="README" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3324" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3356" uniqueCount="369">
   <si>
     <t>feature</t>
   </si>
@@ -1074,6 +1075,21 @@
     <t>ar20d_nonnull</t>
   </si>
   <si>
+    <t>pval</t>
+  </si>
+  <si>
+    <t>sig</t>
+  </si>
+  <si>
+    <t>_z_feat</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>key</t>
   </si>
   <si>
@@ -1098,7 +1114,7 @@
     <t>files_written</t>
   </si>
   <si>
-    <t>2025-08-15 12:56</t>
+    <t>2025-08-15 14:04</t>
   </si>
   <si>
     <t>C:\Users\j1072\sec-risk-sentiment</t>
@@ -1113,7 +1129,7 @@
     <t>AAPL, MSFT, NVDA</t>
   </si>
   <si>
-    <t>signal_shortlist, signal_summary, *_sig, correlations_all, events_all, events_summary</t>
+    <t>signal_shortlist, signal_summary, *_sig, correlations_all, events_all, events_summary, panel_summary</t>
   </si>
 </sst>
 </file>
@@ -3391,6 +3407,82 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>361</v>
+      </c>
+      <c r="B6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A110"/>
@@ -28576,7 +28668,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -28585,64 +28677,175 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>352</v>
       </c>
-      <c r="B2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="D2">
+        <v>0.0052722058640852</v>
+      </c>
+      <c r="E2">
+        <v>0.009076658435748799</v>
+      </c>
+      <c r="F2">
+        <v>0.5613394136973452</v>
+      </c>
+      <c r="G2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3">
+        <v>-0.0224420266992482</v>
+      </c>
+      <c r="E3">
+        <v>0.0218197679023216</v>
+      </c>
+      <c r="F3">
+        <v>0.3037061709352575</v>
+      </c>
+      <c r="G3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D4">
+        <v>-0.0103246330582949</v>
+      </c>
+      <c r="E4">
+        <v>0.008503685992944401</v>
+      </c>
+      <c r="F4">
+        <v>0.2246957157746366</v>
+      </c>
+      <c r="G4" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5">
+        <v>-0.0147647293618283</v>
+      </c>
+      <c r="E5">
+        <v>0.0152433808851551</v>
+      </c>
+      <c r="F5">
+        <v>0.332745109973396</v>
+      </c>
+      <c r="G5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>352</v>
+      </c>
+      <c r="D6">
+        <v>0.0012483691103768</v>
+      </c>
+      <c r="E6">
+        <v>0.0092658140826561</v>
+      </c>
+      <c r="F6">
+        <v>0.8928265493189212</v>
+      </c>
+      <c r="G6" t="s">
         <v>353</v>
       </c>
-      <c r="B3" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7">
+        <v>-0.0158643266549467</v>
+      </c>
+      <c r="E7">
+        <v>0.0185693966282855</v>
+      </c>
+      <c r="F7">
+        <v>0.3929241371003321</v>
+      </c>
+      <c r="G7" t="s">
         <v>354</v>
-      </c>
-      <c r="B4" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>355</v>
-      </c>
-      <c r="B5" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>356</v>
-      </c>
-      <c r="B6" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>357</v>
-      </c>
-      <c r="B7" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>